<commit_message>
First draft and supporting changes
Add sorting details.
</commit_message>
<xml_diff>
--- a/dev-topics-algorithms/dev-topics-nasa-sensor/analysis/PerformanceAnalysis.xlsx
+++ b/dev-topics-algorithms/dev-topics-nasa-sensor/analysis/PerformanceAnalysis.xlsx
@@ -9,12 +9,13 @@
   <sheets>
     <sheet name="raw_4" sheetId="1" r:id="rId1"/>
     <sheet name="Timing" sheetId="2" r:id="rId2"/>
+    <sheet name="Million" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="runTime_4" localSheetId="0">raw_4!$A$1:$F$51</definedName>
     <definedName name="runTime_4" localSheetId="1">Timing!$A$1:$F$51</definedName>
   </definedNames>
-  <calcPr calcId="145621" iterate="1"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -683,11 +684,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="134625536"/>
-        <c:axId val="134624000"/>
+        <c:axId val="125520128"/>
+        <c:axId val="125526784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="134625536"/>
+        <c:axId val="125520128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="15000000"/>
@@ -723,9 +724,10 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134624000"/>
+        <c:crossAx val="125526784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1000000"/>
         <c:dispUnits>
           <c:builtInUnit val="millions"/>
           <c:dispUnitsLbl>
@@ -734,7 +736,7 @@
         </c:dispUnits>
       </c:valAx>
       <c:valAx>
-        <c:axId val="134624000"/>
+        <c:axId val="125526784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -761,7 +763,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" b="1" i="1" baseline="0"/>
-                  <a:t>SEC</a:t>
+                  <a:t>SECS</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US" b="1" i="1"/>
               </a:p>
@@ -774,7 +776,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134625536"/>
+        <c:crossAx val="125520128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1331,11 +1333,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="15225600"/>
-        <c:axId val="15237120"/>
+        <c:axId val="125563264"/>
+        <c:axId val="125565568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="15225600"/>
+        <c:axId val="125563264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="15000000"/>
@@ -1371,9 +1373,10 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="15237120"/>
+        <c:crossAx val="125565568"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1000000"/>
         <c:dispUnits>
           <c:builtInUnit val="millions"/>
           <c:dispUnitsLbl>
@@ -1382,7 +1385,7 @@
         </c:dispUnits>
       </c:valAx>
       <c:valAx>
-        <c:axId val="15237120"/>
+        <c:axId val="125565568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.5"/>
@@ -1428,7 +1431,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="15225600"/>
+        <c:crossAx val="125563264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="5.000000000000001E-2"/>
@@ -1437,6 +1440,265 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Java Map - Area Collection</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Time per Burst</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.6245949020638535E-2"/>
+          <c:y val="1.4220252295930384E-2"/>
+          <c:w val="0.86830206595344239"/>
+          <c:h val="0.8882989652318849"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Timing!$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MonitorExposureByAreaMapped</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Timing!$C$12:$C$17</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Timing!$E$12:$E$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.4393899999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.0297000000000007E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5154900000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.14820340000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.58733259999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5478537000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="125586816"/>
+        <c:axId val="125593088"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="125586816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1000000"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Radiation</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Bursts in Exposure Interval</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="125593088"/>
+        <c:crossesAt val="0"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="100000"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="125593088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2.5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="wordArtVert"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1" i="1" baseline="0"/>
+                  <a:t>Average Burst Time</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US" b="1" i="1" baseline="0"/>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1" i="1" baseline="0"/>
+                  <a:t>US</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" b="1" i="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="out"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="125586816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:minorUnit val="5.000000000000001E-2"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.68139310726910152"/>
+          <c:y val="0.2166715499071071"/>
+          <c:w val="0.28396361146114313"/>
+          <c:h val="3.8362057589273933E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1461,10 +1723,10 @@
       <xdr:rowOff>23813</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>642937</xdr:colOff>
       <xdr:row>76</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>23813</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1510,6 +1772,43 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>207169</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2857,7 +3156,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C42" workbookViewId="0">
+      <selection activeCell="AA70" sqref="AA70"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -3898,4 +4199,19 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>